<commit_message>
add co2 prices excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/CO2_prices.xlsx
+++ b/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/CO2_prices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="values_without_PV" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="values_with_PV" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="values_without_PV" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="values_with_PV" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
integrate EUA prices into output table of CO2 comparison
</commit_message>
<xml_diff>
--- a/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/CO2_prices.xlsx
+++ b/Spine_Projects/03_output_data/03_runs_paper_energy_2024/03_results_comparison/CO2_prices.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,11 @@
           <t>CO2 Equivalents</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CO2 Price [EUA]</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -490,6 +495,9 @@
       <c r="G2" t="n">
         <v>1.340915205159723</v>
       </c>
+      <c r="H2" t="n">
+        <v>24.723125</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -515,6 +523,9 @@
       <c r="G3" t="n">
         <v>1.785671976504156</v>
       </c>
+      <c r="H3" t="n">
+        <v>24.38660287</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -540,6 +551,9 @@
       <c r="G4" t="n">
         <v>1.559842037940293</v>
       </c>
+      <c r="H4" t="n">
+        <v>54.15156951</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -565,6 +579,9 @@
       <c r="G5" t="n">
         <v>1.681234962030197</v>
       </c>
+      <c r="H5" t="n">
+        <v>80.18404545</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -590,6 +607,9 @@
       <c r="G6" t="n">
         <v>1.802800256614671</v>
       </c>
+      <c r="H6" t="n">
+        <v>83.59650224000001</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -614,6 +634,9 @@
       </c>
       <c r="G7" t="n">
         <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>221.0376</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +650,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,6 +689,11 @@
           <t>CO2 Equivalents</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CO2 Price [EUA]</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -691,6 +719,9 @@
       <c r="G2" t="n">
         <v>1.340915205159723</v>
       </c>
+      <c r="H2" t="n">
+        <v>24.723125</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -716,6 +747,9 @@
       <c r="G3" t="n">
         <v>1.785671976504156</v>
       </c>
+      <c r="H3" t="n">
+        <v>24.38660287</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -741,6 +775,9 @@
       <c r="G4" t="n">
         <v>1.559842037940293</v>
       </c>
+      <c r="H4" t="n">
+        <v>54.15156951</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -766,6 +803,9 @@
       <c r="G5" t="n">
         <v>1.681234962030197</v>
       </c>
+      <c r="H5" t="n">
+        <v>80.18404545</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -791,6 +831,9 @@
       <c r="G6" t="n">
         <v>1.802800256614671</v>
       </c>
+      <c r="H6" t="n">
+        <v>83.59650224000001</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -815,6 +858,9 @@
       </c>
       <c r="G7" t="n">
         <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>221.0376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>